<commit_message>
distance penyesuaian terminal multipurpose
</commit_message>
<xml_diff>
--- a/POI/Points_Terminal.xlsx
+++ b/POI/Points_Terminal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semester 7\Skripsi\Data\ArcGIS\git\aoi\POI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A9310B5-82AA-41D5-B50E-495CE8B31E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF777D21-DC94-451C-B87D-32C003EC3708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1278" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="574">
   <si>
     <t>objectid</t>
   </si>
@@ -1742,15 +1742,19 @@
   </si>
   <si>
     <t>Satui Bunati</t>
+  </si>
+  <si>
+    <t>Terminal Multipurpose - Labuan Bajo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.00000"/>
     <numFmt numFmtId="165" formatCode="#,##0.000000"/>
+    <numFmt numFmtId="169" formatCode="#,##0.0000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -1790,11 +1794,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2101,12 +2106,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
       <selection activeCell="H145" sqref="H145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34" customWidth="1"/>
     <col min="8" max="8" width="45.6640625" customWidth="1"/>
@@ -8361,7 +8367,48 @@
       </c>
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C144" s="1"/>
+      <c r="A144">
+        <v>621</v>
+      </c>
+      <c r="B144" s="4">
+        <v>-8.4620847579484195</v>
+      </c>
+      <c r="C144" s="1">
+        <v>119.921630946208</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="E144" t="s">
+        <v>339</v>
+      </c>
+      <c r="F144" t="s">
+        <v>16</v>
+      </c>
+      <c r="G144" t="s">
+        <v>17</v>
+      </c>
+      <c r="H144" t="s">
+        <v>340</v>
+      </c>
+      <c r="I144" t="s">
+        <v>318</v>
+      </c>
+      <c r="J144" t="s">
+        <v>341</v>
+      </c>
+      <c r="K144">
+        <v>53</v>
+      </c>
+      <c r="L144">
+        <v>53.15</v>
+      </c>
+      <c r="M144" t="s">
+        <v>22</v>
+      </c>
+      <c r="N144" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>